<commit_message>
added in vps-1-core : actix-tokio-postgres, grip
</commit_message>
<xml_diff>
--- a/results/vps_1_core.xlsx
+++ b/results/vps_1_core.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fat/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fat/worx/tmp/ws-benchmark/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,12 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>http4s</t>
-  </si>
-  <si>
-    <t>spider-g</t>
   </si>
   <si>
     <t>requests per second</t>
@@ -45,6 +42,15 @@
   </si>
   <si>
     <t>actix-diesel</t>
+  </si>
+  <si>
+    <t>actix-tokio</t>
+  </si>
+  <si>
+    <t>spider-gazelle</t>
+  </si>
+  <si>
+    <t>grip</t>
   </si>
 </sst>
 </file>
@@ -124,9 +130,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,9 +225,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$B$6</c:f>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>http4s</c:v>
                 </c:pt>
@@ -232,17 +238,23 @@
                   <c:v>spring</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>spider-g</c:v>
+                  <c:v>actix-tokio</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>spider-gazelle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>grip</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$6</c:f>
+              <c:f>Sheet1!$C$3:$C$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>502.08</c:v>
                 </c:pt>
@@ -253,7 +265,13 @@
                   <c:v>1029.87</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>3046.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2750.41</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2746.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -268,11 +286,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="2078608224"/>
-        <c:axId val="-1899076128"/>
+        <c:axId val="2119137456"/>
+        <c:axId val="2121553456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2078608224"/>
+        <c:axId val="2119137456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -315,7 +333,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1899076128"/>
+        <c:crossAx val="2121553456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -323,7 +341,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1899076128"/>
+        <c:axId val="2121553456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -343,7 +361,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -374,7 +392,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2078608224"/>
+        <c:crossAx val="2119137456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -501,9 +519,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$B$6</c:f>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>http4s</c:v>
                 </c:pt>
@@ -514,17 +532,23 @@
                   <c:v>spring</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>spider-g</c:v>
+                  <c:v>actix-tokio</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>spider-gazelle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>grip</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$6</c:f>
+              <c:f>Sheet1!$D$3:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>195072.0</c:v>
                 </c:pt>
@@ -535,7 +559,13 @@
                   <c:v>180344.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>3668.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>7660.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7640.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -550,11 +580,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="-2124526224"/>
-        <c:axId val="-1898311952"/>
+        <c:axId val="2121382144"/>
+        <c:axId val="2121378736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2124526224"/>
+        <c:axId val="2121382144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -597,7 +627,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1898311952"/>
+        <c:crossAx val="2121378736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -605,7 +635,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1898311952"/>
+        <c:axId val="2121378736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -656,7 +686,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2124526224"/>
+        <c:crossAx val="2121382144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1839,7 +1869,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>690880</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>10160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1863,13 +1893,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>81280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>701040</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2155,14 +2185,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -2170,73 +2202,103 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <v>502.08</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>195072</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <f>D3/1024</f>
         <v>190.5</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5">
         <v>1796.52</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>5560</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <f>D4/1024</f>
         <v>5.4296875</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
         <v>1029.8699999999999</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>180344</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <f>D5/1024</f>
         <v>176.1171875</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5">
+        <v>3046.2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3668</v>
+      </c>
+      <c r="E6" s="3">
+        <f>D6/1024</f>
+        <v>3.58203125</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5">
         <v>2750.41</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D7" s="4">
         <v>7660</v>
       </c>
-      <c r="E6" s="4">
-        <f>D6/1024</f>
+      <c r="E7" s="3">
+        <f>D7/1024</f>
         <v>7.48046875</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2746.69</v>
+      </c>
+      <c r="D8" s="4">
+        <v>7640</v>
+      </c>
+      <c r="E8" s="3">
+        <f>D8/1024</f>
+        <v>7.4609375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>